<commit_message>
Making ChunkHandler a World satic class
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Ефремов</t>
   </si>
@@ -44,6 +44,30 @@
   <si>
     <t>Транслирование и масштабирование мира
 разделенние оконных и мировых координат</t>
+  </si>
+  <si>
+    <t>Текстуры блоков</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Изменение соотношений размеров блоков</t>
+  </si>
+  <si>
+    <t>Генерация деревьев</t>
+  </si>
+  <si>
+    <t>Привести мировые координаты к размеру блока = 1.0f</t>
+  </si>
+  <si>
+    <t>Пещеры</t>
+  </si>
+  <si>
+    <t>Параметризация генерации мира</t>
+  </si>
+  <si>
+    <t>Хоть какая-то физика воды</t>
   </si>
 </sst>
 </file>
@@ -59,13 +83,25 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -299,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -311,33 +347,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -618,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:F36"/>
+  <dimension ref="C1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,10 +675,11 @@
     <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="7"/>
       <c r="D2" s="5" t="s">
         <v>0</v>
@@ -643,293 +690,315 @@
       <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F3" s="16"/>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>7</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>9</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>10</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>11</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <v>12</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>13</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>14</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>15</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>16</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>17</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>18</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>19</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>20</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>21</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>22</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>23</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>24</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>25</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>26</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>27</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>28</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>29</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>30</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>31</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>32</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>33</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="2">
         <v>34</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Structures ans Tree upd.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Ефремов</t>
   </si>
@@ -44,13 +44,62 @@
   <si>
     <t>Транслирование и масштабирование мира
 разделенние оконных и мировых координат</t>
+  </si>
+  <si>
+    <t>Текстуры блоков</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Изменение соотношений размеров блоков</t>
+  </si>
+  <si>
+    <t>Генерация деревьев</t>
+  </si>
+  <si>
+    <t>Привести мировые координаты к размеру блока = 1.0f</t>
+  </si>
+  <si>
+    <t>Пещеры</t>
+  </si>
+  <si>
+    <t>Параметризация генерации мира</t>
+  </si>
+  <si>
+    <t>Хоть какая-то физика воды</t>
+  </si>
+  <si>
+    <t>Инвентарь</t>
+  </si>
+  <si>
+    <t>Система ломания и подбирания блоков</t>
+  </si>
+  <si>
+    <t>Меню</t>
+  </si>
+  <si>
+    <t>Освещение</t>
+  </si>
+  <si>
+    <t>Текстуру чела</t>
+  </si>
+  <si>
+    <t>Биомы</t>
+  </si>
+  <si>
+    <t>Pathfinding -&gt; мобы</t>
+  </si>
+  <si>
+    <t>GUI(кнопки, регистрация
+ нажатий через события)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,14 +107,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -106,33 +185,61 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -142,105 +249,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -256,17 +264,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -291,6 +288,90 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -299,43 +380,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -618,318 +714,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:F36"/>
+  <dimension ref="C1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" customWidth="1"/>
+    <col min="9" max="9" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="7"/>
-      <c r="D2" s="5" t="s">
+    <row r="1" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="4"/>
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="6">
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="21">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="3:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C4" s="1">
+      <c r="F3" s="13"/>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="22">
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="1">
+      <c r="I4" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="22">
         <v>3</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
+      <c r="D5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="22">
         <v>4</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
+      <c r="D6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="22">
         <v>5</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="22">
         <v>6</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
+      <c r="D8" s="19"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="I8" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="22">
         <v>7</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="1">
+      <c r="D9" s="19"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="I9" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="22">
         <v>8</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="1">
+      <c r="D10" s="19"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="22">
         <v>9</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1">
+      <c r="D11" s="19"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="22">
         <v>10</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="1">
+      <c r="D12" s="19"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="22">
         <v>11</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="1">
+      <c r="D13" s="19"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="22">
         <v>12</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="1">
+      <c r="D14" s="19"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="22">
         <v>13</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="1">
+      <c r="D15" s="19"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="22">
         <v>14</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
+      <c r="C17" s="22">
         <v>15</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="1">
+      <c r="C18" s="22">
         <v>16</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
+      <c r="C19" s="22">
         <v>17</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
+      <c r="C20" s="22">
         <v>18</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
+      <c r="C21" s="22">
         <v>19</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
+      <c r="C22" s="22">
         <v>20</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="1">
+      <c r="C23" s="22">
         <v>21</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="1">
+      <c r="C24" s="22">
         <v>22</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="1">
+      <c r="C25" s="22">
         <v>23</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="1">
+      <c r="C26" s="22">
         <v>24</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="1">
+      <c r="C27" s="22">
         <v>25</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="1">
+      <c r="C28" s="22">
         <v>26</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="1">
+      <c r="C29" s="22">
         <v>27</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="1">
+      <c r="C30" s="22">
         <v>28</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="1">
+      <c r="C31" s="22">
         <v>29</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="1">
+      <c r="C32" s="22">
         <v>30</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="1">
+      <c r="C33" s="22">
         <v>31</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="1">
+      <c r="C34" s="22">
         <v>32</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="1">
+      <c r="C35" s="22">
         <v>33</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="2">
+      <c r="C36" s="23">
         <v>34</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>